<commit_message>
Adicionado imagens ao artigo e simulação na pasta de imagens.
</commit_message>
<xml_diff>
--- a/Cálculo e Simulação/Perdas nas chaves do matricial - Easy 2B.xlsx
+++ b/Cálculo e Simulação/Perdas nas chaves do matricial - Easy 2B.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
   <si>
     <t>Ref: Analytical Modeling of Semiconductor Losses in Matrix Converter</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>Simulação Extrudado 60815 sem ventilação</t>
+  </si>
+  <si>
+    <t>Simulação Extrudado 60815 com 50CFM</t>
   </si>
 </sst>
 </file>
@@ -230,12 +233,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -247,14 +244,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -262,6 +253,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -462,12 +465,12 @@
           </c:val>
         </c:ser>
         <c:bandFmts/>
-        <c:axId val="232480576"/>
-        <c:axId val="232480968"/>
-        <c:axId val="244737672"/>
+        <c:axId val="73630992"/>
+        <c:axId val="73631552"/>
+        <c:axId val="77140656"/>
       </c:surface3DChart>
       <c:catAx>
-        <c:axId val="232480576"/>
+        <c:axId val="73630992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -496,7 +499,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="232480968"/>
+        <c:crossAx val="73631552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -504,7 +507,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="232480968"/>
+        <c:axId val="73631552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -534,12 +537,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="232480576"/>
+        <c:crossAx val="73630992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="244737672"/>
+        <c:axId val="77140656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -548,7 +551,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="232480968"/>
+        <c:crossAx val="73631552"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -760,12 +763,12 @@
           </c:val>
         </c:ser>
         <c:bandFmts/>
-        <c:axId val="503221984"/>
-        <c:axId val="235750032"/>
-        <c:axId val="210596568"/>
+        <c:axId val="200180336"/>
+        <c:axId val="200180896"/>
+        <c:axId val="77141280"/>
       </c:surface3DChart>
       <c:catAx>
-        <c:axId val="503221984"/>
+        <c:axId val="200180336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -794,7 +797,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="235750032"/>
+        <c:crossAx val="200180896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -802,7 +805,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="235750032"/>
+        <c:axId val="200180896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -832,12 +835,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="503221984"/>
+        <c:crossAx val="200180336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="210596568"/>
+        <c:axId val="77141280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -846,7 +849,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="235750032"/>
+        <c:crossAx val="200180896"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -1935,35 +1938,35 @@
         <v>678.82250993908565</v>
       </c>
       <c r="D8">
-        <f>C8</f>
+        <f t="shared" ref="D8:D13" si="0">C8</f>
         <v>678.82250993908565</v>
       </c>
       <c r="E8">
-        <f t="shared" ref="E8:K8" si="0">D8</f>
+        <f t="shared" ref="E8:K8" si="1">D8</f>
         <v>678.82250993908565</v>
       </c>
       <c r="F8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>678.82250993908565</v>
       </c>
       <c r="G8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>678.82250993908565</v>
       </c>
       <c r="H8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>678.82250993908565</v>
       </c>
       <c r="I8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>678.82250993908565</v>
       </c>
       <c r="J8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>678.82250993908565</v>
       </c>
       <c r="K8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>678.82250993908565</v>
       </c>
     </row>
@@ -1975,7 +1978,7 @@
         <v>17</v>
       </c>
       <c r="D9">
-        <f>C9</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="E9">
@@ -1986,11 +1989,11 @@
         <v>24</v>
       </c>
       <c r="G9">
-        <f>F9</f>
+        <f t="shared" ref="G9:H13" si="2">F9</f>
         <v>24</v>
       </c>
       <c r="H9">
-        <f>G9</f>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="I9">
@@ -2013,7 +2016,7 @@
         <v>380</v>
       </c>
       <c r="D10">
-        <f>C10</f>
+        <f t="shared" si="0"/>
         <v>380</v>
       </c>
       <c r="E10">
@@ -2024,11 +2027,11 @@
         <v>380</v>
       </c>
       <c r="G10">
-        <f>F10</f>
+        <f t="shared" si="2"/>
         <v>380</v>
       </c>
       <c r="H10">
-        <f>G10</f>
+        <f t="shared" si="2"/>
         <v>380</v>
       </c>
       <c r="I10">
@@ -2051,7 +2054,7 @@
         <v>0.9</v>
       </c>
       <c r="D11">
-        <f>C11</f>
+        <f t="shared" si="0"/>
         <v>0.9</v>
       </c>
       <c r="E11">
@@ -2062,11 +2065,11 @@
         <v>1.05</v>
       </c>
       <c r="G11">
-        <f>F11</f>
+        <f t="shared" si="2"/>
         <v>1.05</v>
       </c>
       <c r="H11">
-        <f>G11</f>
+        <f t="shared" si="2"/>
         <v>1.05</v>
       </c>
       <c r="I11">
@@ -2089,7 +2092,7 @@
         <v>1</v>
       </c>
       <c r="D12">
-        <f>C12</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E12">
@@ -2100,11 +2103,11 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="G12">
-        <f>F12</f>
+        <f t="shared" si="2"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="H12">
-        <f>G12</f>
+        <f t="shared" si="2"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="I12">
@@ -2128,7 +2131,7 @@
         <v>24.041630560342618</v>
       </c>
       <c r="D13">
-        <f>C13</f>
+        <f t="shared" si="0"/>
         <v>24.041630560342618</v>
       </c>
       <c r="E13">
@@ -2136,19 +2139,19 @@
         <v>24.041630560342618</v>
       </c>
       <c r="F13">
-        <f t="shared" ref="F13:K13" si="1">F9*SQRT(2)</f>
+        <f t="shared" ref="F13:I13" si="3">F9*SQRT(2)</f>
         <v>33.941125496954285</v>
       </c>
       <c r="G13">
-        <f>F13</f>
+        <f t="shared" si="2"/>
         <v>33.941125496954285</v>
       </c>
       <c r="H13">
-        <f>G13</f>
+        <f t="shared" si="2"/>
         <v>33.941125496954285</v>
       </c>
       <c r="I13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>43.840620433565952</v>
       </c>
       <c r="J13">
@@ -2168,33 +2171,33 @@
         <v>1.3636300000000001E-2</v>
       </c>
       <c r="D14">
-        <f t="shared" ref="D14:E15" si="2">C14</f>
+        <f t="shared" ref="D14:E15" si="4">C14</f>
         <v>1.3636300000000001E-2</v>
       </c>
       <c r="E14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1.3636300000000001E-2</v>
       </c>
       <c r="F14">
         <v>1.0714285714285701E-2</v>
       </c>
       <c r="G14">
-        <f t="shared" ref="G14:H14" si="3">F14</f>
+        <f t="shared" ref="G14:H14" si="5">F14</f>
         <v>1.0714285714285701E-2</v>
       </c>
       <c r="H14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.0714285714285701E-2</v>
       </c>
       <c r="I14">
         <v>9.3749999999999997E-3</v>
       </c>
       <c r="J14">
-        <f t="shared" ref="J14:K14" si="4">I14</f>
+        <f t="shared" ref="J14:K14" si="6">I14</f>
         <v>9.3749999999999997E-3</v>
       </c>
       <c r="K14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>9.3749999999999997E-3</v>
       </c>
     </row>
@@ -2206,33 +2209,33 @@
         <v>8.7500000000000008E-3</v>
       </c>
       <c r="D15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8.7500000000000008E-3</v>
       </c>
       <c r="E15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8.7500000000000008E-3</v>
       </c>
       <c r="F15">
         <v>7.9000000000000008E-3</v>
       </c>
       <c r="G15">
-        <f t="shared" ref="G15:H15" si="5">F15</f>
+        <f t="shared" ref="G15:H15" si="7">F15</f>
         <v>7.9000000000000008E-3</v>
       </c>
       <c r="H15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>7.9000000000000008E-3</v>
       </c>
       <c r="I15">
         <v>6.6666666666666602E-3</v>
       </c>
       <c r="J15">
-        <f t="shared" ref="J15:K15" si="6">I15</f>
+        <f t="shared" ref="J15:K15" si="8">I15</f>
         <v>6.6666666666666602E-3</v>
       </c>
       <c r="K15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>6.6666666666666602E-3</v>
       </c>
     </row>
@@ -2286,31 +2289,31 @@
         <v>2.8E-3</v>
       </c>
       <c r="E17">
-        <f t="shared" ref="E17:K17" si="7">D17</f>
+        <f t="shared" ref="E17:K17" si="9">D17</f>
         <v>2.8E-3</v>
       </c>
       <c r="F17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2.8E-3</v>
       </c>
       <c r="G17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2.8E-3</v>
       </c>
       <c r="H17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2.8E-3</v>
       </c>
       <c r="I17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2.8E-3</v>
       </c>
       <c r="J17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2.8E-3</v>
       </c>
       <c r="K17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2.8E-3</v>
       </c>
       <c r="L17" t="s">
@@ -2329,31 +2332,31 @@
         <v>4.1000000000000003E-3</v>
       </c>
       <c r="E18">
-        <f t="shared" ref="E18:K18" si="8">D18</f>
+        <f t="shared" ref="E18:K18" si="10">D18</f>
         <v>4.1000000000000003E-3</v>
       </c>
       <c r="F18">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>4.1000000000000003E-3</v>
       </c>
       <c r="G18">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>4.1000000000000003E-3</v>
       </c>
       <c r="H18">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>4.1000000000000003E-3</v>
       </c>
       <c r="I18">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>4.1000000000000003E-3</v>
       </c>
       <c r="J18">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>4.1000000000000003E-3</v>
       </c>
       <c r="K18">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>4.1000000000000003E-3</v>
       </c>
       <c r="L18" t="s">
@@ -2372,31 +2375,31 @@
         <v>1.5499999999999999E-3</v>
       </c>
       <c r="E19">
-        <f t="shared" ref="E19:K19" si="9">D19</f>
+        <f t="shared" ref="E19:K19" si="11">D19</f>
         <v>1.5499999999999999E-3</v>
       </c>
       <c r="F19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.5499999999999999E-3</v>
       </c>
       <c r="G19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.5499999999999999E-3</v>
       </c>
       <c r="H19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.5499999999999999E-3</v>
       </c>
       <c r="I19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.5499999999999999E-3</v>
       </c>
       <c r="J19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.5499999999999999E-3</v>
       </c>
       <c r="K19">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>1.5499999999999999E-3</v>
       </c>
     </row>
@@ -2412,31 +2415,31 @@
         <v>400</v>
       </c>
       <c r="E20">
-        <f t="shared" ref="E20:K20" si="10">D20</f>
+        <f t="shared" ref="E20:K20" si="12">D20</f>
         <v>400</v>
       </c>
       <c r="F20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>400</v>
       </c>
       <c r="G20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>400</v>
       </c>
       <c r="H20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>400</v>
       </c>
       <c r="I20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>400</v>
       </c>
       <c r="J20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>400</v>
       </c>
       <c r="K20">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>400</v>
       </c>
     </row>
@@ -2452,31 +2455,31 @@
         <v>100</v>
       </c>
       <c r="E21">
-        <f t="shared" ref="E21:K21" si="11">D21</f>
+        <f t="shared" ref="E21:K21" si="13">D21</f>
         <v>100</v>
       </c>
       <c r="F21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>100</v>
       </c>
       <c r="G21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>100</v>
       </c>
       <c r="H21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>100</v>
       </c>
       <c r="I21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>100</v>
       </c>
       <c r="J21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>100</v>
       </c>
       <c r="K21">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>100</v>
       </c>
     </row>
@@ -2486,7 +2489,7 @@
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C24" s="6">
@@ -2518,7 +2521,7 @@
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C25" s="6">
@@ -2558,35 +2561,35 @@
         <v>106.6495731356236</v>
       </c>
       <c r="D26">
-        <f t="shared" ref="D26:E26" si="12">6/PI()*(D11+D12)*D13+3/2*D13*D13*(D14+D15)</f>
+        <f t="shared" ref="D26:E26" si="14">6/PI()*(D11+D12)*D13+3/2*D13*D13*(D14+D15)</f>
         <v>106.6495731356236</v>
       </c>
       <c r="E26">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>106.6495731356236</v>
       </c>
       <c r="F26">
-        <f t="shared" ref="F26:K26" si="13">6/PI()*(F11+F12)*F13+3/2*F13*F13*(F14+F15)</f>
+        <f t="shared" ref="F26:K26" si="15">6/PI()*(F11+F12)*F13+3/2*F13*F13*(F14+F15)</f>
         <v>171.53445145540576</v>
       </c>
       <c r="G26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>171.53445145540576</v>
       </c>
       <c r="H26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>171.53445145540576</v>
       </c>
       <c r="I26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>238.82578502600501</v>
       </c>
       <c r="J26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>238.82578502600501</v>
       </c>
       <c r="K26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>238.82578502600501</v>
       </c>
     </row>
@@ -2599,35 +2602,35 @@
         <v>102.67719548662578</v>
       </c>
       <c r="D27">
-        <f t="shared" ref="D27:E27" si="14">SQRT(3)*24*D16*(D17+D18+D19)*D8*D9/(D20*D21*PI()*PI())</f>
+        <f t="shared" ref="D27:E27" si="16">SQRT(3)*24*D16*(D17+D18+D19)*D8*D9/(D20*D21*PI()*PI())</f>
         <v>205.35439097325155</v>
       </c>
       <c r="E27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>308.0315864598773</v>
       </c>
       <c r="F27">
-        <f t="shared" ref="F27:K27" si="15">SQRT(3)*24*F16*(F17+F18+F19)*F8*F9/(F20*F21*PI()*PI())</f>
+        <f t="shared" ref="F27:K27" si="17">SQRT(3)*24*F16*(F17+F18+F19)*F8*F9/(F20*F21*PI()*PI())</f>
         <v>144.95604068700109</v>
       </c>
       <c r="G27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>289.91208137400218</v>
       </c>
       <c r="H27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>434.86812206100331</v>
       </c>
       <c r="I27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>187.23488588737641</v>
       </c>
       <c r="J27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>374.46977177475281</v>
       </c>
       <c r="K27">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>561.70465766212919</v>
       </c>
     </row>
@@ -2640,35 +2643,35 @@
         <v>209.32676862224938</v>
       </c>
       <c r="D29">
-        <f t="shared" ref="D29:E29" si="16">D26+D27</f>
+        <f t="shared" ref="D29:E29" si="18">D26+D27</f>
         <v>312.00396410887515</v>
       </c>
       <c r="E29">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>414.6811595955009</v>
       </c>
       <c r="F29">
-        <f t="shared" ref="F29:K29" si="17">F26+F27</f>
+        <f t="shared" ref="F29:K29" si="19">F26+F27</f>
         <v>316.49049214240688</v>
       </c>
       <c r="G29">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>461.44653282940794</v>
       </c>
       <c r="H29">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>606.40257351640912</v>
       </c>
       <c r="I29">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>426.06067091338139</v>
       </c>
       <c r="J29">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>613.29555680075782</v>
       </c>
       <c r="K29">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>800.53044268813414</v>
       </c>
     </row>
@@ -2683,35 +2686,35 @@
         <v>0.97921312930638971</v>
       </c>
       <c r="D39" s="1">
-        <f t="shared" ref="D39:K39" si="18">1-D29/$C$3</f>
+        <f t="shared" ref="D39:K39" si="20">1-D29/$C$3</f>
         <v>0.96901692936592887</v>
       </c>
       <c r="E39" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0.95882072942546803</v>
       </c>
       <c r="F39" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0.96857140164527422</v>
       </c>
       <c r="G39" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0.95417676643521188</v>
       </c>
       <c r="H39" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0.93978213122514953</v>
       </c>
       <c r="I39" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0.95769070467097461</v>
       </c>
       <c r="J39" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0.93909763419131087</v>
       </c>
       <c r="K39" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>0.92050456371164702</v>
       </c>
     </row>
@@ -2845,8 +2848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A9:U66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="T19" sqref="T19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2871,13 +2874,13 @@
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="2">
         <v>10000</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="20" t="s">
         <v>37</v>
       </c>
       <c r="F10" s="2">
@@ -2894,11 +2897,11 @@
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="15"/>
+      <c r="B11" s="19"/>
       <c r="C11" s="2">
         <v>20000</v>
       </c>
-      <c r="E11" s="8"/>
+      <c r="E11" s="17"/>
       <c r="F11" s="2">
         <f>Plan1!F29</f>
         <v>316.49049214240688</v>
@@ -2913,11 +2916,11 @@
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="15"/>
+      <c r="B12" s="19"/>
       <c r="C12" s="2">
         <v>30000</v>
       </c>
-      <c r="E12" s="8"/>
+      <c r="E12" s="17"/>
       <c r="F12" s="2">
         <f>Plan1!I29</f>
         <v>426.06067091338139</v>
@@ -2932,16 +2935,16 @@
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="14"/>
-      <c r="E13" s="14"/>
+      <c r="B13" s="12"/>
+      <c r="E13" s="12"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="14"/>
-      <c r="E14" s="14"/>
+      <c r="B14" s="12"/>
+      <c r="E14" s="12"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="14"/>
-      <c r="E15" s="8" t="s">
+      <c r="B15" s="12"/>
+      <c r="E15" s="17" t="s">
         <v>36</v>
       </c>
       <c r="F15" s="2">
@@ -2967,8 +2970,8 @@
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="14"/>
-      <c r="E16" s="8"/>
+      <c r="B16" s="12"/>
+      <c r="E16" s="17"/>
       <c r="F16" s="2">
         <f t="shared" ref="F16:H16" si="1">F11/18</f>
         <v>17.582805119022606</v>
@@ -2992,7 +2995,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E17" s="8"/>
+      <c r="E17" s="17"/>
       <c r="F17" s="2">
         <f t="shared" ref="F17:H17" si="2">F12/18</f>
         <v>23.670037272965633</v>
@@ -3016,10 +3019,10 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E18" s="14"/>
+      <c r="E18" s="12"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E19" s="14"/>
+      <c r="E19" s="12"/>
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
@@ -3028,19 +3031,19 @@
       <c r="C20" s="2">
         <v>125</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E20" s="17" t="s">
         <v>31</v>
       </c>
       <c r="F20" s="3">
-        <f>$C$20-(F15*$C$21)</f>
+        <f t="shared" ref="F20:H22" si="3">$C$20-(F15*$C$21)</f>
         <v>122.09268376913542</v>
       </c>
       <c r="G20" s="3">
-        <f>$C$20-(G15*$C$21)</f>
+        <f t="shared" si="3"/>
         <v>120.66661160959896</v>
       </c>
       <c r="H20" s="3">
-        <f>$C$20-(H15*$C$21)</f>
+        <f t="shared" si="3"/>
         <v>119.24053945006249</v>
       </c>
     </row>
@@ -3051,54 +3054,54 @@
       <c r="C21" s="2">
         <v>0.25</v>
       </c>
-      <c r="E21" s="8"/>
+      <c r="E21" s="17"/>
       <c r="F21" s="3">
-        <f>$C$20-(F16*$C$21)</f>
+        <f t="shared" si="3"/>
         <v>120.60429872024434</v>
       </c>
       <c r="G21" s="3">
-        <f>$C$20-(G16*$C$21)</f>
+        <f t="shared" si="3"/>
         <v>118.59102037736933</v>
       </c>
       <c r="H21" s="3">
-        <f>$C$20-(H16*$C$21)</f>
+        <f t="shared" si="3"/>
         <v>116.57774203449432</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E22" s="8"/>
+      <c r="E22" s="17"/>
       <c r="F22" s="3">
-        <f>$C$20-(F17*$C$21)</f>
+        <f t="shared" si="3"/>
         <v>119.08249068175859</v>
       </c>
       <c r="G22" s="3">
-        <f>$C$20-(G17*$C$21)</f>
+        <f t="shared" si="3"/>
         <v>116.48200615554504</v>
       </c>
       <c r="H22" s="3">
-        <f>$C$20-(H17*$C$21)</f>
+        <f t="shared" si="3"/>
         <v>113.88152162933147</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E23" s="16"/>
+      <c r="E23" s="13"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E24" s="16"/>
+      <c r="E24" s="13"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E25" s="9" t="s">
+      <c r="E25" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -3118,10 +3121,10 @@
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="12">
+      <c r="A27" s="10">
         <v>250</v>
       </c>
-      <c r="B27" s="13">
+      <c r="B27" s="11">
         <v>212</v>
       </c>
       <c r="E27" s="7" t="s">
@@ -3189,40 +3192,40 @@
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="14">
+      <c r="A30" s="12">
         <f>A27-A29</f>
         <v>85</v>
       </c>
-      <c r="B30" s="14">
+      <c r="B30" s="12">
         <f>B27-B29</f>
         <v>95</v>
       </c>
-      <c r="E30" s="12"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="14">
+      <c r="A31" s="12">
         <f>A30/4</f>
         <v>21.25</v>
       </c>
-      <c r="B31" s="14">
+      <c r="B31" s="12">
         <f>B30/4</f>
         <v>23.75</v>
       </c>
-      <c r="E31" s="12"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E32" s="20" t="s">
+      <c r="E32" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
     </row>
     <row r="33" spans="2:21" x14ac:dyDescent="0.25">
       <c r="F33" s="2" t="s">
@@ -3236,7 +3239,7 @@
       </c>
     </row>
     <row r="34" spans="2:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E34" s="8" t="s">
+      <c r="E34" s="17" t="s">
         <v>40</v>
       </c>
       <c r="F34" s="2">
@@ -3246,7 +3249,7 @@
       <c r="H34" s="2"/>
     </row>
     <row r="35" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="E35" s="8"/>
+      <c r="E35" s="17"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2">
@@ -3254,7 +3257,7 @@
       </c>
     </row>
     <row r="36" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="E36" s="8"/>
+      <c r="E36" s="17"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2">
         <v>161</v>
@@ -3264,359 +3267,390 @@
       </c>
     </row>
     <row r="38" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="E38" s="14"/>
+      <c r="E38" s="12"/>
       <c r="P38" s="6"/>
     </row>
     <row r="39" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="E39" s="14"/>
-      <c r="M39" s="13"/>
-      <c r="N39" s="13"/>
-      <c r="O39" s="13"/>
-      <c r="P39" s="12"/>
-      <c r="Q39" s="13"/>
-      <c r="R39" s="13"/>
-      <c r="S39" s="13"/>
-      <c r="T39" s="13"/>
-      <c r="U39" s="13"/>
+      <c r="E39" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="M39" s="11"/>
+      <c r="N39" s="11"/>
+      <c r="O39" s="11"/>
+      <c r="P39" s="10"/>
+      <c r="Q39" s="11"/>
+      <c r="R39" s="11"/>
+      <c r="S39" s="11"/>
+      <c r="T39" s="11"/>
+      <c r="U39" s="11"/>
     </row>
     <row r="40" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="M40" s="13"/>
-      <c r="N40" s="13"/>
-      <c r="O40" s="12"/>
-      <c r="P40" s="12"/>
-      <c r="Q40" s="12"/>
-      <c r="R40" s="12"/>
-      <c r="S40" s="12"/>
-      <c r="T40" s="12"/>
-      <c r="U40" s="12"/>
+      <c r="F40" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="M40" s="11"/>
+      <c r="N40" s="11"/>
+      <c r="O40" s="10"/>
+      <c r="P40" s="10"/>
+      <c r="Q40" s="10"/>
+      <c r="R40" s="10"/>
+      <c r="S40" s="10"/>
+      <c r="T40" s="10"/>
+      <c r="U40" s="10"/>
     </row>
     <row r="41" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B41" s="5"/>
+      <c r="E41" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
-      <c r="M41" s="13"/>
-      <c r="N41" s="13"/>
-      <c r="O41" s="12"/>
-      <c r="P41" s="19"/>
-      <c r="Q41" s="18"/>
-      <c r="R41" s="18"/>
-      <c r="S41" s="18"/>
-      <c r="T41" s="18"/>
-      <c r="U41" s="18"/>
+      <c r="M41" s="11"/>
+      <c r="N41" s="11"/>
+      <c r="O41" s="10"/>
+      <c r="P41" s="15"/>
+      <c r="Q41" s="14"/>
+      <c r="R41" s="14"/>
+      <c r="S41" s="14"/>
+      <c r="T41" s="14"/>
+      <c r="U41" s="14"/>
     </row>
     <row r="42" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B42" s="5"/>
+      <c r="E42" s="17"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
-      <c r="M42" s="13"/>
-      <c r="N42" s="13"/>
-      <c r="O42" s="12"/>
-      <c r="P42" s="19"/>
-      <c r="Q42" s="18"/>
-      <c r="R42" s="18"/>
-      <c r="S42" s="18"/>
-      <c r="T42" s="18"/>
-      <c r="U42" s="18"/>
+      <c r="M42" s="11"/>
+      <c r="N42" s="11"/>
+      <c r="O42" s="10"/>
+      <c r="P42" s="15"/>
+      <c r="Q42" s="14"/>
+      <c r="R42" s="14"/>
+      <c r="S42" s="14"/>
+      <c r="T42" s="14"/>
+      <c r="U42" s="14"/>
     </row>
     <row r="43" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B43" s="5"/>
+      <c r="E43" s="17"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2">
+        <v>127</v>
+      </c>
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
-      <c r="M43" s="13"/>
-      <c r="N43" s="13"/>
-      <c r="O43" s="12"/>
-      <c r="P43" s="19"/>
-      <c r="Q43" s="18"/>
-      <c r="R43" s="18"/>
-      <c r="S43" s="18"/>
-      <c r="T43" s="18"/>
-      <c r="U43" s="18"/>
+      <c r="M43" s="11"/>
+      <c r="N43" s="11"/>
+      <c r="O43" s="10"/>
+      <c r="P43" s="15"/>
+      <c r="Q43" s="14"/>
+      <c r="R43" s="14"/>
+      <c r="S43" s="14"/>
+      <c r="T43" s="14"/>
+      <c r="U43" s="14"/>
     </row>
     <row r="44" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B44" s="5"/>
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
-      <c r="M44" s="13"/>
-      <c r="N44" s="13"/>
-      <c r="O44" s="12"/>
-      <c r="P44" s="19"/>
-      <c r="Q44" s="18"/>
-      <c r="R44" s="18"/>
-      <c r="S44" s="18"/>
-      <c r="T44" s="18"/>
-      <c r="U44" s="18"/>
+      <c r="M44" s="11"/>
+      <c r="N44" s="11"/>
+      <c r="O44" s="10"/>
+      <c r="P44" s="15"/>
+      <c r="Q44" s="14"/>
+      <c r="R44" s="14"/>
+      <c r="S44" s="14"/>
+      <c r="T44" s="14"/>
+      <c r="U44" s="14"/>
     </row>
     <row r="45" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B45" s="5"/>
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
-      <c r="M45" s="13"/>
-      <c r="N45" s="13"/>
-      <c r="O45" s="12"/>
-      <c r="P45" s="19"/>
-      <c r="Q45" s="18"/>
-      <c r="R45" s="18"/>
-      <c r="S45" s="18"/>
-      <c r="T45" s="18"/>
-      <c r="U45" s="18"/>
+      <c r="M45" s="11"/>
+      <c r="N45" s="11"/>
+      <c r="O45" s="10"/>
+      <c r="P45" s="15"/>
+      <c r="Q45" s="14"/>
+      <c r="R45" s="14"/>
+      <c r="S45" s="14"/>
+      <c r="T45" s="14"/>
+      <c r="U45" s="14"/>
     </row>
     <row r="46" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B46" s="5"/>
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
-      <c r="M46" s="13"/>
-      <c r="N46" s="13"/>
-      <c r="O46" s="12"/>
-      <c r="P46" s="19"/>
-      <c r="Q46" s="18"/>
-      <c r="R46" s="18"/>
-      <c r="S46" s="18"/>
-      <c r="T46" s="18"/>
-      <c r="U46" s="18"/>
+      <c r="M46" s="11"/>
+      <c r="N46" s="11"/>
+      <c r="O46" s="10"/>
+      <c r="P46" s="15"/>
+      <c r="Q46" s="14"/>
+      <c r="R46" s="14"/>
+      <c r="S46" s="14"/>
+      <c r="T46" s="14"/>
+      <c r="U46" s="14"/>
     </row>
     <row r="47" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B47" s="5"/>
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
-      <c r="M47" s="13"/>
-      <c r="N47" s="13"/>
-      <c r="O47" s="12"/>
-      <c r="P47" s="19"/>
-      <c r="Q47" s="18"/>
-      <c r="R47" s="18"/>
-      <c r="S47" s="18"/>
-      <c r="T47" s="18"/>
-      <c r="U47" s="18"/>
+      <c r="M47" s="11"/>
+      <c r="N47" s="11"/>
+      <c r="O47" s="10"/>
+      <c r="P47" s="15"/>
+      <c r="Q47" s="14"/>
+      <c r="R47" s="14"/>
+      <c r="S47" s="14"/>
+      <c r="T47" s="14"/>
+      <c r="U47" s="14"/>
     </row>
     <row r="48" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="M48" s="13"/>
-      <c r="N48" s="13"/>
-      <c r="O48" s="13"/>
-      <c r="P48" s="12"/>
-      <c r="Q48" s="13"/>
-      <c r="R48" s="13"/>
-      <c r="S48" s="13"/>
-      <c r="T48" s="13"/>
-      <c r="U48" s="13"/>
+      <c r="M48" s="11"/>
+      <c r="N48" s="11"/>
+      <c r="O48" s="11"/>
+      <c r="P48" s="10"/>
+      <c r="Q48" s="11"/>
+      <c r="R48" s="11"/>
+      <c r="S48" s="11"/>
+      <c r="T48" s="11"/>
+      <c r="U48" s="11"/>
     </row>
     <row r="49" spans="9:21" x14ac:dyDescent="0.25">
-      <c r="I49" s="11"/>
-      <c r="J49" s="11"/>
-      <c r="M49" s="13"/>
-      <c r="N49" s="13"/>
-      <c r="O49" s="12"/>
-      <c r="P49" s="12"/>
-      <c r="Q49" s="12"/>
-      <c r="R49" s="12"/>
-      <c r="S49" s="12"/>
-      <c r="T49" s="12"/>
-      <c r="U49" s="12"/>
+      <c r="I49" s="9"/>
+      <c r="J49" s="9"/>
+      <c r="M49" s="11"/>
+      <c r="N49" s="11"/>
+      <c r="O49" s="10"/>
+      <c r="P49" s="10"/>
+      <c r="Q49" s="10"/>
+      <c r="R49" s="10"/>
+      <c r="S49" s="10"/>
+      <c r="T49" s="10"/>
+      <c r="U49" s="10"/>
     </row>
     <row r="50" spans="9:21" x14ac:dyDescent="0.25">
-      <c r="I50" s="12"/>
-      <c r="J50" s="12"/>
-      <c r="M50" s="13"/>
-      <c r="N50" s="13"/>
-      <c r="O50" s="12"/>
-      <c r="P50" s="19"/>
-      <c r="Q50" s="18"/>
-      <c r="R50" s="18"/>
-      <c r="S50" s="18"/>
-      <c r="T50" s="18"/>
-      <c r="U50" s="18"/>
+      <c r="I50" s="10"/>
+      <c r="J50" s="10"/>
+      <c r="M50" s="11"/>
+      <c r="N50" s="11"/>
+      <c r="O50" s="10"/>
+      <c r="P50" s="15"/>
+      <c r="Q50" s="14"/>
+      <c r="R50" s="14"/>
+      <c r="S50" s="14"/>
+      <c r="T50" s="14"/>
+      <c r="U50" s="14"/>
     </row>
     <row r="51" spans="9:21" x14ac:dyDescent="0.25">
-      <c r="I51" s="13"/>
-      <c r="J51" s="13"/>
-      <c r="M51" s="13"/>
-      <c r="N51" s="13"/>
-      <c r="O51" s="12"/>
-      <c r="P51" s="19"/>
-      <c r="Q51" s="18"/>
-      <c r="R51" s="18"/>
-      <c r="S51" s="18"/>
-      <c r="T51" s="18"/>
-      <c r="U51" s="18"/>
+      <c r="I51" s="11"/>
+      <c r="J51" s="11"/>
+      <c r="M51" s="11"/>
+      <c r="N51" s="11"/>
+      <c r="O51" s="10"/>
+      <c r="P51" s="15"/>
+      <c r="Q51" s="14"/>
+      <c r="R51" s="14"/>
+      <c r="S51" s="14"/>
+      <c r="T51" s="14"/>
+      <c r="U51" s="14"/>
     </row>
     <row r="52" spans="9:21" x14ac:dyDescent="0.25">
-      <c r="I52" s="13"/>
-      <c r="J52" s="13"/>
-      <c r="M52" s="13"/>
-      <c r="N52" s="13"/>
-      <c r="O52" s="12"/>
-      <c r="P52" s="19"/>
-      <c r="Q52" s="18"/>
-      <c r="R52" s="18"/>
-      <c r="S52" s="18"/>
-      <c r="T52" s="18"/>
-      <c r="U52" s="18"/>
+      <c r="I52" s="11"/>
+      <c r="J52" s="11"/>
+      <c r="M52" s="11"/>
+      <c r="N52" s="11"/>
+      <c r="O52" s="10"/>
+      <c r="P52" s="15"/>
+      <c r="Q52" s="14"/>
+      <c r="R52" s="14"/>
+      <c r="S52" s="14"/>
+      <c r="T52" s="14"/>
+      <c r="U52" s="14"/>
     </row>
     <row r="53" spans="9:21" x14ac:dyDescent="0.25">
-      <c r="I53" s="13"/>
-      <c r="J53" s="13"/>
-      <c r="M53" s="13"/>
-      <c r="N53" s="13"/>
-      <c r="O53" s="12"/>
-      <c r="P53" s="19"/>
-      <c r="Q53" s="18"/>
-      <c r="R53" s="18"/>
-      <c r="S53" s="18"/>
-      <c r="T53" s="18"/>
-      <c r="U53" s="18"/>
+      <c r="I53" s="11"/>
+      <c r="J53" s="11"/>
+      <c r="M53" s="11"/>
+      <c r="N53" s="11"/>
+      <c r="O53" s="10"/>
+      <c r="P53" s="15"/>
+      <c r="Q53" s="14"/>
+      <c r="R53" s="14"/>
+      <c r="S53" s="14"/>
+      <c r="T53" s="14"/>
+      <c r="U53" s="14"/>
     </row>
     <row r="54" spans="9:21" x14ac:dyDescent="0.25">
-      <c r="I54" s="13"/>
-      <c r="J54" s="13"/>
-      <c r="M54" s="13"/>
-      <c r="N54" s="13"/>
-      <c r="O54" s="12"/>
-      <c r="P54" s="19"/>
-      <c r="Q54" s="18"/>
-      <c r="R54" s="18"/>
-      <c r="S54" s="18"/>
-      <c r="T54" s="18"/>
-      <c r="U54" s="18"/>
+      <c r="I54" s="11"/>
+      <c r="J54" s="11"/>
+      <c r="M54" s="11"/>
+      <c r="N54" s="11"/>
+      <c r="O54" s="10"/>
+      <c r="P54" s="15"/>
+      <c r="Q54" s="14"/>
+      <c r="R54" s="14"/>
+      <c r="S54" s="14"/>
+      <c r="T54" s="14"/>
+      <c r="U54" s="14"/>
     </row>
     <row r="55" spans="9:21" x14ac:dyDescent="0.25">
-      <c r="I55" s="13"/>
-      <c r="J55" s="13"/>
-      <c r="M55" s="13"/>
-      <c r="N55" s="13"/>
-      <c r="O55" s="12"/>
-      <c r="P55" s="19"/>
-      <c r="Q55" s="18"/>
-      <c r="R55" s="18"/>
-      <c r="S55" s="18"/>
-      <c r="T55" s="18"/>
-      <c r="U55" s="18"/>
+      <c r="I55" s="11"/>
+      <c r="J55" s="11"/>
+      <c r="M55" s="11"/>
+      <c r="N55" s="11"/>
+      <c r="O55" s="10"/>
+      <c r="P55" s="15"/>
+      <c r="Q55" s="14"/>
+      <c r="R55" s="14"/>
+      <c r="S55" s="14"/>
+      <c r="T55" s="14"/>
+      <c r="U55" s="14"/>
     </row>
     <row r="56" spans="9:21" x14ac:dyDescent="0.25">
-      <c r="I56" s="13"/>
-      <c r="J56" s="13"/>
-      <c r="M56" s="13"/>
-      <c r="N56" s="13"/>
-      <c r="O56" s="12"/>
-      <c r="P56" s="19"/>
-      <c r="Q56" s="18"/>
-      <c r="R56" s="18"/>
-      <c r="S56" s="18"/>
-      <c r="T56" s="18"/>
-      <c r="U56" s="18"/>
+      <c r="I56" s="11"/>
+      <c r="J56" s="11"/>
+      <c r="M56" s="11"/>
+      <c r="N56" s="11"/>
+      <c r="O56" s="10"/>
+      <c r="P56" s="15"/>
+      <c r="Q56" s="14"/>
+      <c r="R56" s="14"/>
+      <c r="S56" s="14"/>
+      <c r="T56" s="14"/>
+      <c r="U56" s="14"/>
     </row>
     <row r="57" spans="9:21" x14ac:dyDescent="0.25">
-      <c r="I57" s="13"/>
-      <c r="J57" s="13"/>
-      <c r="M57" s="13"/>
-      <c r="N57" s="13"/>
-      <c r="O57" s="13"/>
-      <c r="P57" s="13"/>
-      <c r="Q57" s="13"/>
-      <c r="R57" s="13"/>
-      <c r="S57" s="13"/>
-      <c r="T57" s="13"/>
-      <c r="U57" s="13"/>
+      <c r="I57" s="11"/>
+      <c r="J57" s="11"/>
+      <c r="M57" s="11"/>
+      <c r="N57" s="11"/>
+      <c r="O57" s="11"/>
+      <c r="P57" s="11"/>
+      <c r="Q57" s="11"/>
+      <c r="R57" s="11"/>
+      <c r="S57" s="11"/>
+      <c r="T57" s="11"/>
+      <c r="U57" s="11"/>
     </row>
     <row r="58" spans="9:21" x14ac:dyDescent="0.25">
-      <c r="M58" s="13"/>
-      <c r="N58" s="12"/>
-      <c r="O58" s="13"/>
-      <c r="P58" s="12"/>
-      <c r="Q58" s="12"/>
-      <c r="R58" s="12"/>
-      <c r="S58" s="12"/>
-      <c r="T58" s="12"/>
-      <c r="U58" s="13"/>
+      <c r="M58" s="11"/>
+      <c r="N58" s="10"/>
+      <c r="O58" s="11"/>
+      <c r="P58" s="10"/>
+      <c r="Q58" s="10"/>
+      <c r="R58" s="10"/>
+      <c r="S58" s="10"/>
+      <c r="T58" s="10"/>
+      <c r="U58" s="11"/>
     </row>
     <row r="59" spans="9:21" x14ac:dyDescent="0.25">
-      <c r="M59" s="13"/>
-      <c r="N59" s="12"/>
-      <c r="O59" s="19"/>
-      <c r="P59" s="18"/>
-      <c r="Q59" s="18"/>
-      <c r="R59" s="18"/>
-      <c r="S59" s="18"/>
-      <c r="T59" s="18"/>
-      <c r="U59" s="13"/>
+      <c r="M59" s="11"/>
+      <c r="N59" s="10"/>
+      <c r="O59" s="15"/>
+      <c r="P59" s="14"/>
+      <c r="Q59" s="14"/>
+      <c r="R59" s="14"/>
+      <c r="S59" s="14"/>
+      <c r="T59" s="14"/>
+      <c r="U59" s="11"/>
     </row>
     <row r="60" spans="9:21" x14ac:dyDescent="0.25">
-      <c r="M60" s="13"/>
-      <c r="N60" s="12"/>
-      <c r="O60" s="19"/>
-      <c r="P60" s="18"/>
-      <c r="Q60" s="18"/>
-      <c r="R60" s="18"/>
-      <c r="S60" s="18"/>
-      <c r="T60" s="18"/>
-      <c r="U60" s="13"/>
+      <c r="M60" s="11"/>
+      <c r="N60" s="10"/>
+      <c r="O60" s="15"/>
+      <c r="P60" s="14"/>
+      <c r="Q60" s="14"/>
+      <c r="R60" s="14"/>
+      <c r="S60" s="14"/>
+      <c r="T60" s="14"/>
+      <c r="U60" s="11"/>
     </row>
     <row r="61" spans="9:21" x14ac:dyDescent="0.25">
-      <c r="M61" s="13"/>
-      <c r="N61" s="12"/>
-      <c r="O61" s="19"/>
-      <c r="P61" s="18"/>
-      <c r="Q61" s="18"/>
-      <c r="R61" s="18"/>
-      <c r="S61" s="18"/>
-      <c r="T61" s="18"/>
-      <c r="U61" s="13"/>
+      <c r="M61" s="11"/>
+      <c r="N61" s="10"/>
+      <c r="O61" s="15"/>
+      <c r="P61" s="14"/>
+      <c r="Q61" s="14"/>
+      <c r="R61" s="14"/>
+      <c r="S61" s="14"/>
+      <c r="T61" s="14"/>
+      <c r="U61" s="11"/>
     </row>
     <row r="62" spans="9:21" x14ac:dyDescent="0.25">
-      <c r="M62" s="13"/>
-      <c r="N62" s="12"/>
-      <c r="O62" s="19"/>
-      <c r="P62" s="18"/>
-      <c r="Q62" s="18"/>
-      <c r="R62" s="18"/>
-      <c r="S62" s="18"/>
-      <c r="T62" s="18"/>
-      <c r="U62" s="13"/>
+      <c r="M62" s="11"/>
+      <c r="N62" s="10"/>
+      <c r="O62" s="15"/>
+      <c r="P62" s="14"/>
+      <c r="Q62" s="14"/>
+      <c r="R62" s="14"/>
+      <c r="S62" s="14"/>
+      <c r="T62" s="14"/>
+      <c r="U62" s="11"/>
     </row>
     <row r="63" spans="9:21" x14ac:dyDescent="0.25">
-      <c r="M63" s="13"/>
-      <c r="N63" s="12"/>
-      <c r="O63" s="19"/>
-      <c r="P63" s="18"/>
-      <c r="Q63" s="18"/>
-      <c r="R63" s="18"/>
-      <c r="S63" s="18"/>
-      <c r="T63" s="18"/>
-      <c r="U63" s="13"/>
+      <c r="M63" s="11"/>
+      <c r="N63" s="10"/>
+      <c r="O63" s="15"/>
+      <c r="P63" s="14"/>
+      <c r="Q63" s="14"/>
+      <c r="R63" s="14"/>
+      <c r="S63" s="14"/>
+      <c r="T63" s="14"/>
+      <c r="U63" s="11"/>
     </row>
     <row r="64" spans="9:21" x14ac:dyDescent="0.25">
-      <c r="M64" s="13"/>
-      <c r="N64" s="12"/>
-      <c r="O64" s="19"/>
-      <c r="P64" s="18"/>
-      <c r="Q64" s="18"/>
-      <c r="R64" s="18"/>
-      <c r="S64" s="18"/>
-      <c r="T64" s="18"/>
-      <c r="U64" s="13"/>
+      <c r="M64" s="11"/>
+      <c r="N64" s="10"/>
+      <c r="O64" s="15"/>
+      <c r="P64" s="14"/>
+      <c r="Q64" s="14"/>
+      <c r="R64" s="14"/>
+      <c r="S64" s="14"/>
+      <c r="T64" s="14"/>
+      <c r="U64" s="11"/>
     </row>
     <row r="65" spans="13:21" x14ac:dyDescent="0.25">
-      <c r="M65" s="13"/>
-      <c r="N65" s="12"/>
-      <c r="O65" s="19"/>
-      <c r="P65" s="18"/>
-      <c r="Q65" s="18"/>
-      <c r="R65" s="18"/>
-      <c r="S65" s="18"/>
-      <c r="T65" s="18"/>
-      <c r="U65" s="13"/>
+      <c r="M65" s="11"/>
+      <c r="N65" s="10"/>
+      <c r="O65" s="15"/>
+      <c r="P65" s="14"/>
+      <c r="Q65" s="14"/>
+      <c r="R65" s="14"/>
+      <c r="S65" s="14"/>
+      <c r="T65" s="14"/>
+      <c r="U65" s="11"/>
     </row>
     <row r="66" spans="13:21" x14ac:dyDescent="0.25">
-      <c r="M66" s="13"/>
-      <c r="N66" s="11"/>
-      <c r="O66" s="11"/>
-      <c r="P66" s="11"/>
-      <c r="Q66" s="11"/>
-      <c r="R66" s="11"/>
-      <c r="S66" s="11"/>
-      <c r="T66" s="11"/>
-      <c r="U66" s="13"/>
+      <c r="M66" s="11"/>
+      <c r="N66" s="9"/>
+      <c r="O66" s="9"/>
+      <c r="P66" s="9"/>
+      <c r="Q66" s="9"/>
+      <c r="R66" s="9"/>
+      <c r="S66" s="9"/>
+      <c r="T66" s="9"/>
+      <c r="U66" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="E41:E43"/>
     <mergeCell ref="E20:E22"/>
     <mergeCell ref="E15:E17"/>
     <mergeCell ref="E34:E36"/>

</xml_diff>

<commit_message>
Finalizado artigo. Adicionado calculo das temperaturas de junção.
</commit_message>
<xml_diff>
--- a/Cálculo e Simulação/Perdas nas chaves do matricial - Easy 2B.xlsx
+++ b/Cálculo e Simulação/Perdas nas chaves do matricial - Easy 2B.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="2"/>
+    <workbookView minimized="1" xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="48">
   <si>
     <t>Ref: Analytical Modeling of Semiconductor Losses in Matrix Converter</t>
   </si>
@@ -145,6 +145,21 @@
   </si>
   <si>
     <t>Simulação Extrudado 60815 com 50CFM</t>
+  </si>
+  <si>
+    <t>Tj (ºC)</t>
+  </si>
+  <si>
+    <t>Simulação Hollowfin com 50CFm</t>
+  </si>
+  <si>
+    <t>Simulação Hollowfin sem ventilação</t>
+  </si>
+  <si>
+    <t>Simulação Hollowfin com 25CFM</t>
+  </si>
+  <si>
+    <t>Simulação Hollowfin com 10CFM</t>
   </si>
 </sst>
 </file>
@@ -465,12 +480,12 @@
           </c:val>
         </c:ser>
         <c:bandFmts/>
-        <c:axId val="73630992"/>
-        <c:axId val="73631552"/>
-        <c:axId val="77140656"/>
+        <c:axId val="199027296"/>
+        <c:axId val="199027856"/>
+        <c:axId val="52499088"/>
       </c:surface3DChart>
       <c:catAx>
-        <c:axId val="73630992"/>
+        <c:axId val="199027296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -499,7 +514,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73631552"/>
+        <c:crossAx val="199027856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -507,7 +522,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="73631552"/>
+        <c:axId val="199027856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -537,12 +552,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73630992"/>
+        <c:crossAx val="199027296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="77140656"/>
+        <c:axId val="52499088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -551,7 +566,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73631552"/>
+        <c:crossAx val="199027856"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -763,12 +778,12 @@
           </c:val>
         </c:ser>
         <c:bandFmts/>
-        <c:axId val="200180336"/>
-        <c:axId val="200180896"/>
-        <c:axId val="77141280"/>
+        <c:axId val="199121072"/>
+        <c:axId val="199121632"/>
+        <c:axId val="52499712"/>
       </c:surface3DChart>
       <c:catAx>
-        <c:axId val="200180336"/>
+        <c:axId val="199121072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -797,7 +812,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="200180896"/>
+        <c:crossAx val="199121632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -805,7 +820,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="200180896"/>
+        <c:axId val="199121632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -835,12 +850,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="200180336"/>
+        <c:crossAx val="199121072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="77141280"/>
+        <c:axId val="52499712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -849,7 +864,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="200180896"/>
+        <c:crossAx val="199121632"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -2846,10 +2861,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A9:U66"/>
+  <dimension ref="A9:U68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="H69" sqref="H69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3036,15 +3051,15 @@
       </c>
       <c r="F20" s="3">
         <f t="shared" ref="F20:H22" si="3">$C$20-(F15*$C$21)</f>
-        <v>122.09268376913542</v>
+        <v>119.18536753827085</v>
       </c>
       <c r="G20" s="3">
         <f t="shared" si="3"/>
-        <v>120.66661160959896</v>
+        <v>116.33322321919792</v>
       </c>
       <c r="H20" s="3">
         <f t="shared" si="3"/>
-        <v>119.24053945006249</v>
+        <v>113.48107890012497</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -3052,35 +3067,35 @@
         <v>30</v>
       </c>
       <c r="C21" s="2">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="3">
         <f t="shared" si="3"/>
-        <v>120.60429872024434</v>
+        <v>116.2085974404887</v>
       </c>
       <c r="G21" s="3">
         <f t="shared" si="3"/>
-        <v>118.59102037736933</v>
+        <v>112.18204075473867</v>
       </c>
       <c r="H21" s="3">
         <f t="shared" si="3"/>
-        <v>116.57774203449432</v>
+        <v>108.15548406898864</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E22" s="17"/>
       <c r="F22" s="3">
         <f t="shared" si="3"/>
-        <v>119.08249068175859</v>
+        <v>113.16498136351719</v>
       </c>
       <c r="G22" s="3">
         <f t="shared" si="3"/>
-        <v>116.48200615554504</v>
+        <v>107.96401231109006</v>
       </c>
       <c r="H22" s="3">
         <f t="shared" si="3"/>
-        <v>113.88152162933147</v>
+        <v>102.76304325866295</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
@@ -3297,7 +3312,15 @@
       <c r="H40" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="M40" s="11"/>
+      <c r="K40" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L40" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M40" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="N40" s="11"/>
       <c r="O40" s="10"/>
       <c r="P40" s="10"/>
@@ -3312,12 +3335,31 @@
       <c r="E41" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
+      <c r="F41" s="2">
+        <v>71.2</v>
+      </c>
+      <c r="G41" s="2">
+        <v>81.8</v>
+      </c>
+      <c r="H41" s="2">
+        <v>90.7</v>
+      </c>
       <c r="I41" s="4"/>
-      <c r="J41" s="4"/>
-      <c r="M41" s="11"/>
+      <c r="J41" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="K41" s="2">
+        <f>F41+J15*$C$21</f>
+        <v>77.2</v>
+      </c>
+      <c r="L41" s="2">
+        <f t="shared" ref="L41:M41" si="4">G41+K15*$C$21</f>
+        <v>90.8</v>
+      </c>
+      <c r="M41" s="2">
+        <f t="shared" si="4"/>
+        <v>102.2</v>
+      </c>
       <c r="N41" s="11"/>
       <c r="O41" s="10"/>
       <c r="P41" s="15"/>
@@ -3330,12 +3372,29 @@
     <row r="42" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B42" s="5"/>
       <c r="E42" s="17"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
+      <c r="F42" s="2">
+        <v>81.8</v>
+      </c>
+      <c r="G42" s="2">
+        <v>95.9</v>
+      </c>
+      <c r="H42" s="2">
+        <v>110</v>
+      </c>
       <c r="I42" s="4"/>
-      <c r="J42" s="4"/>
-      <c r="M42" s="11"/>
+      <c r="J42" s="17"/>
+      <c r="K42" s="2">
+        <f t="shared" ref="K42:K43" si="5">F42+J16*$C$21</f>
+        <v>90.8</v>
+      </c>
+      <c r="L42" s="2">
+        <f t="shared" ref="L42:L43" si="6">G42+K16*$C$21</f>
+        <v>108.9</v>
+      </c>
+      <c r="M42" s="2">
+        <f t="shared" ref="M42:M43" si="7">H42+L16*$C$21</f>
+        <v>127</v>
+      </c>
       <c r="N42" s="11"/>
       <c r="O42" s="10"/>
       <c r="P42" s="15"/>
@@ -3348,14 +3407,29 @@
     <row r="43" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B43" s="5"/>
       <c r="E43" s="17"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
+      <c r="F43" s="2">
+        <v>92.4</v>
+      </c>
+      <c r="G43" s="2">
+        <v>110</v>
+      </c>
       <c r="H43" s="2">
+        <v>129</v>
+      </c>
+      <c r="I43" s="4"/>
+      <c r="J43" s="17"/>
+      <c r="K43" s="2">
+        <f t="shared" si="5"/>
+        <v>104.4</v>
+      </c>
+      <c r="L43" s="2">
+        <f t="shared" si="6"/>
         <v>127</v>
       </c>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
-      <c r="M43" s="11"/>
+      <c r="M43" s="2">
+        <f t="shared" si="7"/>
+        <v>151.5</v>
+      </c>
       <c r="N43" s="11"/>
       <c r="O43" s="10"/>
       <c r="P43" s="15"/>
@@ -3395,8 +3469,12 @@
     </row>
     <row r="46" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B46" s="5"/>
-      <c r="I46" s="4"/>
-      <c r="J46" s="4"/>
+      <c r="E46" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
       <c r="M46" s="11"/>
       <c r="N46" s="11"/>
       <c r="O46" s="10"/>
@@ -3409,9 +3487,24 @@
     </row>
     <row r="47" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B47" s="5"/>
-      <c r="I47" s="4"/>
-      <c r="J47" s="4"/>
-      <c r="M47" s="11"/>
+      <c r="F47" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L47" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M47" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="N47" s="11"/>
       <c r="O47" s="10"/>
       <c r="P47" s="15"/>
@@ -3422,7 +3515,34 @@
       <c r="U47" s="14"/>
     </row>
     <row r="48" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="M48" s="11"/>
+      <c r="E48" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="F48" s="2">
+        <v>55.7</v>
+      </c>
+      <c r="G48" s="2">
+        <v>58.5</v>
+      </c>
+      <c r="H48" s="2">
+        <v>60.9</v>
+      </c>
+      <c r="I48" s="4"/>
+      <c r="J48" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="K48" s="2">
+        <f>F48+J15*$C$21</f>
+        <v>61.7</v>
+      </c>
+      <c r="L48" s="2">
+        <f t="shared" ref="L48:M50" si="8">G48+K15*$C$21</f>
+        <v>67.5</v>
+      </c>
+      <c r="M48" s="2">
+        <f t="shared" si="8"/>
+        <v>72.400000000000006</v>
+      </c>
       <c r="N48" s="11"/>
       <c r="O48" s="11"/>
       <c r="P48" s="10"/>
@@ -3432,10 +3552,31 @@
       <c r="T48" s="11"/>
       <c r="U48" s="11"/>
     </row>
-    <row r="49" spans="9:21" x14ac:dyDescent="0.25">
-      <c r="I49" s="9"/>
-      <c r="J49" s="9"/>
-      <c r="M49" s="11"/>
+    <row r="49" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="E49" s="17"/>
+      <c r="F49" s="2">
+        <v>58.5</v>
+      </c>
+      <c r="G49" s="2">
+        <v>62.3</v>
+      </c>
+      <c r="H49" s="2">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="I49" s="4"/>
+      <c r="J49" s="17"/>
+      <c r="K49" s="2">
+        <f t="shared" ref="K49:K50" si="9">F49+J16*$C$21</f>
+        <v>67.5</v>
+      </c>
+      <c r="L49" s="2">
+        <f t="shared" si="8"/>
+        <v>75.3</v>
+      </c>
+      <c r="M49" s="2">
+        <f t="shared" si="8"/>
+        <v>83.1</v>
+      </c>
       <c r="N49" s="11"/>
       <c r="O49" s="10"/>
       <c r="P49" s="10"/>
@@ -3445,10 +3586,31 @@
       <c r="T49" s="10"/>
       <c r="U49" s="10"/>
     </row>
-    <row r="50" spans="9:21" x14ac:dyDescent="0.25">
-      <c r="I50" s="10"/>
-      <c r="J50" s="10"/>
-      <c r="M50" s="11"/>
+    <row r="50" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="E50" s="17"/>
+      <c r="F50" s="2">
+        <v>61.4</v>
+      </c>
+      <c r="G50" s="2">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="H50" s="2">
+        <v>71.3</v>
+      </c>
+      <c r="I50" s="4"/>
+      <c r="J50" s="17"/>
+      <c r="K50" s="2">
+        <f t="shared" si="9"/>
+        <v>73.400000000000006</v>
+      </c>
+      <c r="L50" s="2">
+        <f t="shared" si="8"/>
+        <v>83.1</v>
+      </c>
+      <c r="M50" s="2">
+        <f t="shared" si="8"/>
+        <v>93.8</v>
+      </c>
       <c r="N50" s="11"/>
       <c r="O50" s="10"/>
       <c r="P50" s="15"/>
@@ -3458,7 +3620,7 @@
       <c r="T50" s="14"/>
       <c r="U50" s="14"/>
     </row>
-    <row r="51" spans="9:21" x14ac:dyDescent="0.25">
+    <row r="51" spans="5:21" x14ac:dyDescent="0.25">
       <c r="I51" s="11"/>
       <c r="J51" s="11"/>
       <c r="M51" s="11"/>
@@ -3471,9 +3633,13 @@
       <c r="T51" s="14"/>
       <c r="U51" s="14"/>
     </row>
-    <row r="52" spans="9:21" x14ac:dyDescent="0.25">
-      <c r="I52" s="11"/>
-      <c r="J52" s="11"/>
+    <row r="52" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="E52" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F52" s="11"/>
+      <c r="G52" s="11"/>
+      <c r="H52" s="11"/>
       <c r="M52" s="11"/>
       <c r="N52" s="11"/>
       <c r="O52" s="10"/>
@@ -3484,10 +3650,25 @@
       <c r="T52" s="14"/>
       <c r="U52" s="14"/>
     </row>
-    <row r="53" spans="9:21" x14ac:dyDescent="0.25">
-      <c r="I53" s="11"/>
-      <c r="J53" s="11"/>
-      <c r="M53" s="11"/>
+    <row r="53" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="F53" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K53" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L53" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M53" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="N53" s="11"/>
       <c r="O53" s="10"/>
       <c r="P53" s="15"/>
@@ -3497,10 +3678,31 @@
       <c r="T53" s="14"/>
       <c r="U53" s="14"/>
     </row>
-    <row r="54" spans="9:21" x14ac:dyDescent="0.25">
-      <c r="I54" s="11"/>
-      <c r="J54" s="11"/>
-      <c r="M54" s="11"/>
+    <row r="54" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="E54" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2">
+        <v>120</v>
+      </c>
+      <c r="H54" s="2"/>
+      <c r="I54" s="4"/>
+      <c r="J54" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="K54" s="2">
+        <f>F54+J15*$C$21</f>
+        <v>6</v>
+      </c>
+      <c r="L54" s="2">
+        <f t="shared" ref="L54:M54" si="10">G54+K15*$C$21</f>
+        <v>129</v>
+      </c>
+      <c r="M54" s="2">
+        <f t="shared" si="10"/>
+        <v>11.5</v>
+      </c>
       <c r="N54" s="11"/>
       <c r="O54" s="10"/>
       <c r="P54" s="15"/>
@@ -3510,10 +3712,27 @@
       <c r="T54" s="14"/>
       <c r="U54" s="14"/>
     </row>
-    <row r="55" spans="9:21" x14ac:dyDescent="0.25">
-      <c r="I55" s="11"/>
-      <c r="J55" s="11"/>
-      <c r="M55" s="11"/>
+    <row r="55" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="E55" s="17"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2">
+        <v>162</v>
+      </c>
+      <c r="I55" s="4"/>
+      <c r="J55" s="17"/>
+      <c r="K55" s="2">
+        <f t="shared" ref="K55:K56" si="11">F55+J16*$C$21</f>
+        <v>9</v>
+      </c>
+      <c r="L55" s="2">
+        <f t="shared" ref="L55:L56" si="12">G55+K16*$C$21</f>
+        <v>13</v>
+      </c>
+      <c r="M55" s="2">
+        <f t="shared" ref="M55:M56" si="13">H55+L16*$C$21</f>
+        <v>179</v>
+      </c>
       <c r="N55" s="11"/>
       <c r="O55" s="10"/>
       <c r="P55" s="15"/>
@@ -3523,10 +3742,25 @@
       <c r="T55" s="14"/>
       <c r="U55" s="14"/>
     </row>
-    <row r="56" spans="9:21" x14ac:dyDescent="0.25">
-      <c r="I56" s="11"/>
-      <c r="J56" s="11"/>
-      <c r="M56" s="11"/>
+    <row r="56" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="E56" s="17"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="17"/>
+      <c r="K56" s="2">
+        <f t="shared" si="11"/>
+        <v>12</v>
+      </c>
+      <c r="L56" s="2">
+        <f t="shared" si="12"/>
+        <v>17</v>
+      </c>
+      <c r="M56" s="2">
+        <f t="shared" si="13"/>
+        <v>22.5</v>
+      </c>
       <c r="N56" s="11"/>
       <c r="O56" s="10"/>
       <c r="P56" s="15"/>
@@ -3536,7 +3770,7 @@
       <c r="T56" s="14"/>
       <c r="U56" s="14"/>
     </row>
-    <row r="57" spans="9:21" x14ac:dyDescent="0.25">
+    <row r="57" spans="5:21" x14ac:dyDescent="0.25">
       <c r="I57" s="11"/>
       <c r="J57" s="11"/>
       <c r="M57" s="11"/>
@@ -3549,7 +3783,13 @@
       <c r="T57" s="11"/>
       <c r="U57" s="11"/>
     </row>
-    <row r="58" spans="9:21" x14ac:dyDescent="0.25">
+    <row r="58" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="E58" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F58" s="11"/>
+      <c r="G58" s="11"/>
+      <c r="H58" s="11"/>
       <c r="M58" s="11"/>
       <c r="N58" s="10"/>
       <c r="O58" s="11"/>
@@ -3560,8 +3800,25 @@
       <c r="T58" s="10"/>
       <c r="U58" s="11"/>
     </row>
-    <row r="59" spans="9:21" x14ac:dyDescent="0.25">
-      <c r="M59" s="11"/>
+    <row r="59" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="F59" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K59" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L59" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M59" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="N59" s="10"/>
       <c r="O59" s="15"/>
       <c r="P59" s="14"/>
@@ -3571,8 +3828,29 @@
       <c r="T59" s="14"/>
       <c r="U59" s="11"/>
     </row>
-    <row r="60" spans="9:21" x14ac:dyDescent="0.25">
-      <c r="M60" s="11"/>
+    <row r="60" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="E60" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="4"/>
+      <c r="J60" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="K60" s="2">
+        <f>F60+J15*$C$21</f>
+        <v>6</v>
+      </c>
+      <c r="L60" s="2">
+        <f t="shared" ref="L60:M60" si="14">G60+K15*$C$21</f>
+        <v>9</v>
+      </c>
+      <c r="M60" s="2">
+        <f t="shared" si="14"/>
+        <v>11.5</v>
+      </c>
       <c r="N60" s="10"/>
       <c r="O60" s="15"/>
       <c r="P60" s="14"/>
@@ -3582,8 +3860,25 @@
       <c r="T60" s="14"/>
       <c r="U60" s="11"/>
     </row>
-    <row r="61" spans="9:21" x14ac:dyDescent="0.25">
-      <c r="M61" s="11"/>
+    <row r="61" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="E61" s="17"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+      <c r="I61" s="4"/>
+      <c r="J61" s="17"/>
+      <c r="K61" s="2">
+        <f t="shared" ref="K61:K62" si="15">F61+J16*$C$21</f>
+        <v>9</v>
+      </c>
+      <c r="L61" s="2">
+        <f t="shared" ref="L61:L62" si="16">G61+K16*$C$21</f>
+        <v>13</v>
+      </c>
+      <c r="M61" s="2">
+        <f t="shared" ref="M61:M62" si="17">H61+L16*$C$21</f>
+        <v>17</v>
+      </c>
       <c r="N61" s="10"/>
       <c r="O61" s="15"/>
       <c r="P61" s="14"/>
@@ -3593,8 +3888,27 @@
       <c r="T61" s="14"/>
       <c r="U61" s="11"/>
     </row>
-    <row r="62" spans="9:21" x14ac:dyDescent="0.25">
-      <c r="M62" s="11"/>
+    <row r="62" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="E62" s="17"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
+      <c r="H62" s="2">
+        <v>84.1</v>
+      </c>
+      <c r="I62" s="4"/>
+      <c r="J62" s="17"/>
+      <c r="K62" s="2">
+        <f t="shared" si="15"/>
+        <v>12</v>
+      </c>
+      <c r="L62" s="2">
+        <f t="shared" si="16"/>
+        <v>17</v>
+      </c>
+      <c r="M62" s="2">
+        <f t="shared" si="17"/>
+        <v>106.6</v>
+      </c>
       <c r="N62" s="10"/>
       <c r="O62" s="15"/>
       <c r="P62" s="14"/>
@@ -3604,7 +3918,7 @@
       <c r="T62" s="14"/>
       <c r="U62" s="11"/>
     </row>
-    <row r="63" spans="9:21" x14ac:dyDescent="0.25">
+    <row r="63" spans="5:21" x14ac:dyDescent="0.25">
       <c r="M63" s="11"/>
       <c r="N63" s="10"/>
       <c r="O63" s="15"/>
@@ -3615,7 +3929,13 @@
       <c r="T63" s="14"/>
       <c r="U63" s="11"/>
     </row>
-    <row r="64" spans="9:21" x14ac:dyDescent="0.25">
+    <row r="64" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="E64" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="F64" s="11"/>
+      <c r="G64" s="11"/>
+      <c r="H64" s="11"/>
       <c r="M64" s="11"/>
       <c r="N64" s="10"/>
       <c r="O64" s="15"/>
@@ -3626,8 +3946,25 @@
       <c r="T64" s="14"/>
       <c r="U64" s="11"/>
     </row>
-    <row r="65" spans="13:21" x14ac:dyDescent="0.25">
-      <c r="M65" s="11"/>
+    <row r="65" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="F65" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K65" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L65" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M65" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="N65" s="10"/>
       <c r="O65" s="15"/>
       <c r="P65" s="14"/>
@@ -3637,8 +3974,29 @@
       <c r="T65" s="14"/>
       <c r="U65" s="11"/>
     </row>
-    <row r="66" spans="13:21" x14ac:dyDescent="0.25">
-      <c r="M66" s="11"/>
+    <row r="66" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="E66" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
+      <c r="H66" s="2"/>
+      <c r="I66" s="4"/>
+      <c r="J66" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="K66" s="2">
+        <f>F66+J15*$C$21</f>
+        <v>6</v>
+      </c>
+      <c r="L66" s="2">
+        <f t="shared" ref="L66:M68" si="18">G66+K15*$C$21</f>
+        <v>9</v>
+      </c>
+      <c r="M66" s="2">
+        <f t="shared" si="18"/>
+        <v>11.5</v>
+      </c>
       <c r="N66" s="9"/>
       <c r="O66" s="9"/>
       <c r="P66" s="9"/>
@@ -3648,15 +4006,66 @@
       <c r="T66" s="9"/>
       <c r="U66" s="11"/>
     </row>
+    <row r="67" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="E67" s="17"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
+      <c r="H67" s="2"/>
+      <c r="I67" s="4"/>
+      <c r="J67" s="17"/>
+      <c r="K67" s="2">
+        <f t="shared" ref="K67:K68" si="19">F67+J16*$C$21</f>
+        <v>9</v>
+      </c>
+      <c r="L67" s="2">
+        <f t="shared" si="18"/>
+        <v>13</v>
+      </c>
+      <c r="M67" s="2">
+        <f t="shared" si="18"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="68" spans="5:21" x14ac:dyDescent="0.25">
+      <c r="E68" s="17"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="2">
+        <v>116</v>
+      </c>
+      <c r="I68" s="4"/>
+      <c r="J68" s="17"/>
+      <c r="K68" s="2">
+        <f t="shared" si="19"/>
+        <v>12</v>
+      </c>
+      <c r="L68" s="2">
+        <f t="shared" si="18"/>
+        <v>17</v>
+      </c>
+      <c r="M68" s="2">
+        <f t="shared" si="18"/>
+        <v>138.5</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="16">
+    <mergeCell ref="E54:E56"/>
+    <mergeCell ref="J54:J56"/>
+    <mergeCell ref="E60:E62"/>
+    <mergeCell ref="J60:J62"/>
+    <mergeCell ref="E66:E68"/>
+    <mergeCell ref="J66:J68"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="J41:J43"/>
+    <mergeCell ref="E48:E50"/>
+    <mergeCell ref="J48:J50"/>
     <mergeCell ref="E41:E43"/>
     <mergeCell ref="E20:E22"/>
     <mergeCell ref="E15:E17"/>
     <mergeCell ref="E34:E36"/>
     <mergeCell ref="E25:H25"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="E10:E12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>